<commit_message>
header-banner by Kha, no responsive yet
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saocu\Desktop\BC51_Nhom6_CapstoneBootstrap-Diner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2976A2AE-A0C7-4DDE-A819-80208D31670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C81B0D-28D5-4573-821E-3550622EC0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9859029C-D30C-41D5-81E4-E6DB4BED5778}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7785" xr2:uid="{9859029C-D30C-41D5-81E4-E6DB4BED5778}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -72,6 +61,15 @@
   </si>
   <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>Nhật Kha</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Chưa responsive</t>
   </si>
 </sst>
 </file>
@@ -302,26 +300,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -349,9 +332,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -386,6 +366,18 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -705,201 +697,226 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="13"/>
+      <c r="B4" s="23">
+        <v>45061</v>
+      </c>
+      <c r="C4" s="23">
+        <v>45062</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="13"/>
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23">
+        <v>45061</v>
+      </c>
+      <c r="C5" s="23">
+        <v>45062</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="13"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="13"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="13"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="13"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="13"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="13"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="13"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="13"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="13"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Categories by Kha, non-responsive
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saocu\Desktop\BC51_Nhom6_CapstoneBootstrap-Diner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA37241-A874-4384-AF2D-C3A7F37566FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C98AAA4-3EB7-44BC-A664-42DD12AEFEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7785" xr2:uid="{9859029C-D30C-41D5-81E4-E6DB4BED5778}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Banner</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Chưa responsive</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,16 +819,28 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="14"/>
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="23">
+        <v>45063</v>
+      </c>
+      <c r="C8" s="23">
+        <v>45064</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>

</xml_diff>

<commit_message>
Update: introVid, Posts, backToTop
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saocu\Desktop\BC51_Nhom6_CapstoneBootstrap-Diner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435F7171-C15C-4E80-8778-706EE6714720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AD2C12-D13F-425B-8E73-CCF52A696BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7785" xr2:uid="{9859029C-D30C-41D5-81E4-E6DB4BED5778}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Overview</t>
+  </si>
+  <si>
+    <t>Introvid</t>
+  </si>
+  <si>
+    <t>Posts</t>
   </si>
 </sst>
 </file>
@@ -711,12 +717,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2624A084-BDD8-4BC5-AA00-15653D921CC8}">
   <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -844,21 +851,11 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="23">
-        <v>45065</v>
-      </c>
-      <c r="C9" s="23">
-        <v>45065</v>
-      </c>
-      <c r="D9" s="27">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
@@ -867,7 +864,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="23">
         <v>45065</v>
@@ -888,11 +885,21 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="14"/>
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="23">
+        <v>45065</v>
+      </c>
+      <c r="C11" s="23">
+        <v>45065</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="19"/>
@@ -900,11 +907,21 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="23">
+        <v>45068</v>
+      </c>
+      <c r="C12" s="23">
+        <v>45068</v>
+      </c>
+      <c r="D12" s="27">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="19"/>
@@ -912,11 +929,21 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="14"/>
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="23">
+        <v>45069</v>
+      </c>
+      <c r="C13" s="23">
+        <v>45069</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="19"/>

</xml_diff>